<commit_message>
Added data, started building script to clean Anabat header files and matching coordinates
</commit_message>
<xml_diff>
--- a/data/Fieldwork 2014 - inventory JM.xlsx
+++ b/data/Fieldwork 2014 - inventory JM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Site</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Annfield</t>
   </si>
   <si>
-    <t>data V1?</t>
-  </si>
-  <si>
     <t>Ferrygate</t>
   </si>
   <si>
@@ -73,6 +70,15 @@
   </si>
   <si>
     <t>Birds V2</t>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t>BATS</t>
+  </si>
+  <si>
+    <t>BIRDS</t>
   </si>
 </sst>
 </file>
@@ -82,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +99,20 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,12 +138,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,164 +460,157 @@
     <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>41827</v>
       </c>
-      <c r="C2" s="3">
-        <v>41864</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="5">
+        <v>41877</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41830</v>
+      </c>
+      <c r="C3" s="5">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41831</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5" s="1">
         <v>41828</v>
       </c>
-      <c r="C3" s="3">
-        <v>41863</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>41830</v>
-      </c>
-      <c r="C4" s="3">
-        <v>41864</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41831</v>
-      </c>
-      <c r="C5" s="3">
-        <v>41863</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="5">
+        <v>41877</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>41842</v>
       </c>
-      <c r="C6" s="3">
-        <v>41865</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="5">
+        <v>41877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="1">
+        <v>41842</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41843</v>
-      </c>
-      <c r="C7" s="3">
-        <v>41865</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>41849</v>
       </c>
-      <c r="C8" s="3">
-        <v>41869</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="5">
+        <v>41879</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>41850</v>
       </c>
-      <c r="C9" s="3">
-        <v>41869</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="5">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>41857</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="5">
         <v>41856</v>
       </c>
-      <c r="C10" s="3">
-        <v>41870</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" s="5">
+        <v>41882</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
-        <v>41856</v>
-      </c>
-      <c r="C11" s="3">
-        <v>41870</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" s="5">
+        <v>41855</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="5">
+        <v>41857</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
         <v>41855</v>
       </c>
-      <c r="C12" s="3">
-        <v>41871</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3">
-        <v>41855</v>
-      </c>
-      <c r="C13" s="3">
-        <v>41871</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
-        <v>41855</v>
-      </c>
-      <c r="C14" s="3">
-        <v>41871</v>
+      <c r="C14" s="5">
+        <v>41878</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -605,10 +621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +639,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,14 +652,17 @@
       <c r="B2" s="1">
         <v>41852</v>
       </c>
-      <c r="C2" s="4">
-        <v>41877</v>
+      <c r="C2" s="7">
+        <v>41874</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <v>41837</v>
+      </c>
       <c r="C3" s="4">
         <v>41878</v>
       </c>
@@ -683,51 +702,51 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>41814</v>
       </c>
-      <c r="C7" s="4">
-        <v>41873</v>
+      <c r="C7" s="7">
+        <v>41871</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>41823</v>
       </c>
-      <c r="C8" s="4">
-        <v>41873</v>
+      <c r="C8" s="7">
+        <v>41871</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>41835</v>
       </c>
-      <c r="C9" s="4">
-        <v>41879</v>
+      <c r="C9" s="7">
+        <v>41876</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>41820</v>
       </c>
-      <c r="C10" s="4">
-        <v>41876</v>
+      <c r="C10" s="7">
+        <v>41873</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>41820</v>
@@ -738,7 +757,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>41837</v>
@@ -749,24 +768,29 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>41835</v>
       </c>
-      <c r="C13" s="4">
-        <v>41880</v>
+      <c r="C13" s="7">
+        <v>41876</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>41837</v>
       </c>
       <c r="C14" s="4">
         <v>41879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>